<commit_message>
updated POB | added some code comments
</commit_message>
<xml_diff>
--- a/documents/06-Tagesberichte/Aktivitäten Gruppe 4.xlsx
+++ b/documents/06-Tagesberichte/Aktivitäten Gruppe 4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="03.05.17" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
   <si>
     <t>Tätigkeit</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Klassendiagramme anfertigen</t>
+  </si>
+  <si>
+    <t>07:45-14:45</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1075,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E4" s="6">
         <v>50</v>
@@ -1089,7 +1092,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E5" s="6">
         <v>75</v>
@@ -1141,7 +1144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>